<commit_message>
Feat: ajout test e2e onglets decription et personnalisation (#44)
* Feat: Ajout test e2e onglet description

* Feat: ajout tests e2e onglet personalisation

* Feat: update xlsx for tests

Co-authored-by: Vincent Lainé <vincent.laine.utc@gmail.com>
</commit_message>
<xml_diff>
--- a/cypress/fixtures/TEMPLATE_CHATBOT-ERREUR.xlsx
+++ b/cypress/fixtures/TEMPLATE_CHATBOT-ERREUR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jean\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laine\Documents\beta.gouv\fabrique-chatbot-front\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAC0550-280B-4FB3-8483-D70D0AE555FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F105E0B0-D2C0-4309-8E3B-B7BC0E322C0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{585389C5-6A76-482F-A969-368084FBEB95}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{585389C5-6A76-482F-A969-368084FBEB95}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Lien</t>
   </si>
   <si>
-    <t>get_started</t>
-  </si>
-  <si>
     <t>Je peut vous éclairer sur le fonctionnement de la Fabrique à Chatbots, vous n'avez qu'à me poser la question 😊</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Si vous ne souhaitez pas que je me présente, il suffit de supprimer l'ID "get_started"</t>
   </si>
   <si>
-    <t>out_of_scope</t>
-  </si>
-  <si>
     <t>Je suis la phrase par défaut quand je ne sais pas répondre à une question 😢. Mais je m'améliore vite 🧐.</t>
   </si>
   <si>
@@ -193,6 +187,12 @@
   </si>
   <si>
     <t>Erreur 2 question (Pas de type)</t>
+  </si>
+  <si>
+    <t>phrase_presentation</t>
+  </si>
+  <si>
+    <t>phrase_hors_sujet</t>
   </si>
 </sst>
 </file>
@@ -591,20 +591,20 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E22" sqref="E22"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="53.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="74.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="53.265625" customWidth="1"/>
+    <col min="4" max="4" width="20.1328125" customWidth="1"/>
+    <col min="5" max="5" width="74.73046875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="3.86328125" style="1" customWidth="1"/>
     <col min="7" max="7" width="74" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -624,265 +624,265 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
       <c r="D8" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="4" t="s">
+    </row>
+    <row r="14" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4" t="s">
+    <row r="15" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
         <v>49</v>
       </c>
-      <c r="D21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="E22" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>